<commit_message>
custom css for all page
</commit_message>
<xml_diff>
--- a/webtooth/static/import/plantilla-pacientes.xlsx
+++ b/webtooth/static/import/plantilla-pacientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MIS-PROYECTOS\PYTHON\practicas_django\proyectoDjango\webtooth\webtooth\static\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7AD57-B4D8-451F-8ECC-AACD03B050E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C8F853-0E3B-4E1A-8A0F-219D926E96E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,13 +49,13 @@
     <t>opr</t>
   </si>
   <si>
-    <t>Ejemplo de lista de pacientes: Nota Los campos Nombre y Apellido Paterno son son obligatorios</t>
-  </si>
-  <si>
     <t>Nombre(s) *</t>
   </si>
   <si>
     <t>Apellido Paterno (*)</t>
+  </si>
+  <si>
+    <t>Ejemplo de lista de pacientes: Nota Los campos Nombre y Apellido Paterno son obligatorios</t>
   </si>
 </sst>
 </file>
@@ -104,10 +104,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -442,36 +442,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update plantilla import patient
</commit_message>
<xml_diff>
--- a/webtooth/static/import/plantilla-pacientes.xlsx
+++ b/webtooth/static/import/plantilla-pacientes.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MIS-PROYECTOS\PYTHON\practicas_django\proyectoDjango\webtooth\webtooth\static\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EXGUTA\PROYECTOS\WEBTOOTH\webtooth\webtooth\static\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C8F853-0E3B-4E1A-8A0F-219D926E96E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,9 +27,6 @@
     <t>Teléfono</t>
   </si>
   <si>
-    <t>Estado</t>
-  </si>
-  <si>
     <t>RFC</t>
   </si>
   <si>
@@ -56,12 +52,15 @@
   </si>
   <si>
     <t>Ejemplo de lista de pacientes: Nota Los campos Nombre y Apellido Paterno son obligatorios</t>
+  </si>
+  <si>
+    <t>Estado(Activo/Inactivo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -71,12 +70,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,14 +103,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -424,142 +425,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="3" width="29.6640625" customWidth="1"/>
-    <col min="4" max="4" width="33.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="3" customWidth="1"/>
+    <col min="2" max="3" width="29.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="5:5">
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="5:5">
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="5:5">
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="5:5">
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="5:5">
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="5:5">
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="5:5">
-      <c r="E26" s="1"/>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>